<commit_message>
Revisão/atualização de dados da Abordagem, Creas, Centro Pop e Cadastro Único (pessoas, atendimentos, ra's e rma); sugestão de ggplot para lista 4 (estimativa de pop rua por RA com IC de 95%).
</commit_message>
<xml_diff>
--- a/as_beneficios_geacaf_mes.xlsx
+++ b/as_beneficios_geacaf_mes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hernany Castro\OneDrive\Área de Trabalho\ajuste_dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hernany Castro\OneDrive\Área de Trabalho\CREAS\creas_r\gith_transito\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5E42E4-E893-449E-A76B-97702A59B895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25E10E9-7305-4E8D-A563-45D4AB1E8DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{91FEA251-11F4-4596-963D-26ACD2BA8456}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>jan</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>mes</t>
+  </si>
+  <si>
+    <t>ano</t>
   </si>
 </sst>
 </file>
@@ -616,16 +619,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E23EB1E9-FBA1-497B-A22E-BEDEF1729F55}">
-  <dimension ref="B1:C15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:3" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:3" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
@@ -633,7 +639,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2023</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -641,7 +650,10 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2023</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -649,7 +661,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2023</v>
+      </c>
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -657,7 +672,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2023</v>
+      </c>
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
@@ -665,7 +683,10 @@
         <v>335</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2023</v>
+      </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
@@ -673,7 +694,10 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2023</v>
+      </c>
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
@@ -681,7 +705,10 @@
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2023</v>
+      </c>
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
@@ -689,7 +716,10 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2023</v>
+      </c>
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
@@ -697,7 +727,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2023</v>
+      </c>
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
@@ -705,7 +738,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2023</v>
+      </c>
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
@@ -713,7 +749,10 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2023</v>
+      </c>
       <c r="B13" s="7" t="s">
         <v>10</v>
       </c>
@@ -721,7 +760,10 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2023</v>
+      </c>
       <c r="B14" s="9" t="s">
         <v>11</v>
       </c>
@@ -729,7 +771,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>